<commit_message>
update; runall orders works
</commit_message>
<xml_diff>
--- a/P1 source datasheet.xlsx
+++ b/P1 source datasheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_T-P1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainuser\Desktop\Revature\Yu_T-P1-3NF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AE018A-AFCC-4BF2-BE94-5E5E50B5A7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91681C0D-3DE7-4E67-9AA8-F596626A16A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21680" yWindow="240" windowWidth="16130" windowHeight="8360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21660" yWindow="1700" windowWidth="16130" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clients" sheetId="7" r:id="rId1"/>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886C8C2-8B3D-42FB-84DE-6A63F66F5732}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -742,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B814752-2C54-4B73-B6B1-BA6FA8C353A6}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>